<commit_message>
Update epu_news_indices.xlsx - 2026-01-05
</commit_message>
<xml_diff>
--- a/data/epu_news_indices.xlsx
+++ b/data/epu_news_indices.xlsx
@@ -458,7 +458,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Generated: 2026-01-05 01:39:05</t>
+          <t>Generated: 2026-01-05 11:44:56</t>
         </is>
       </c>
     </row>
@@ -16682,13 +16682,13 @@
     </row>
     <row r="307">
       <c r="A307" s="4" t="n">
-        <v>46025</v>
+        <v>46026</v>
       </c>
       <c r="B307" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C307" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D307" t="n">
         <v>0</v>
@@ -16712,7 +16712,7 @@
         <v>0</v>
       </c>
       <c r="K307" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L307" t="n">
         <v>0</v>
@@ -16721,13 +16721,13 @@
         <v>0</v>
       </c>
       <c r="N307" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O307" t="n">
         <v>0</v>
       </c>
       <c r="P307" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q307" t="n">
         <v>0</v>
@@ -19183,10 +19183,10 @@
         <v>46021</v>
       </c>
       <c r="B48" t="n">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C48" t="n">
-        <v>3.571428571428571</v>
+        <v>0</v>
       </c>
       <c r="D48" t="n">
         <v>0</v>
@@ -19210,7 +19210,7 @@
         <v>0</v>
       </c>
       <c r="K48" t="n">
-        <v>3.571428571428571</v>
+        <v>0</v>
       </c>
       <c r="L48" t="n">
         <v>0</v>
@@ -19219,13 +19219,13 @@
         <v>0</v>
       </c>
       <c r="N48" t="n">
-        <v>3.571428571428571</v>
+        <v>0</v>
       </c>
       <c r="O48" t="n">
         <v>0</v>
       </c>
       <c r="P48" t="n">
-        <v>3.571428571428571</v>
+        <v>0</v>
       </c>
       <c r="Q48" t="n">
         <v>0</v>
@@ -19932,10 +19932,10 @@
         <v>46023</v>
       </c>
       <c r="B15" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C15" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -19959,7 +19959,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
         <v>0</v>
@@ -19968,13 +19968,13 @@
         <v>0</v>
       </c>
       <c r="N15" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O15" t="n">
         <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="n">
         <v>0</v>

</xml_diff>